<commit_message>
Committing changes to the other Rent Change Project folders and files
</commit_message>
<xml_diff>
--- a/Output Files/Forecasts/All Forecast Methodologies Forecasts (Annual).xlsx
+++ b/Output Files/Forecasts/All Forecast Methodologies Forecasts (Annual).xlsx
@@ -467,7 +467,7 @@
         <v>-0.02420028559071752</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.01348965056240559</v>
+        <v>0.001144417328760028</v>
       </c>
       <c r="D2" t="n">
         <v>-0.02901628607596651</v>
@@ -481,7 +481,7 @@
         <v>-0.02617844399237158</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.01054771896451712</v>
+        <v>0.005653401836752892</v>
       </c>
       <c r="D3" t="n">
         <v>-0.04081823951669225</v>
@@ -495,7 +495,7 @@
         <v>-0.02727115102760983</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.003087596269324422</v>
+        <v>0.008702149614691734</v>
       </c>
       <c r="D4" t="n">
         <v>-0.03376379393821899</v>
@@ -509,7 +509,7 @@
         <v>-0.02787474711165487</v>
       </c>
       <c r="C5" t="n">
-        <v>0.007572321686893702</v>
+        <v>0.01114099565893412</v>
       </c>
       <c r="D5" t="n">
         <v>-0.0160126003287473</v>
@@ -523,7 +523,7 @@
         <v>-0.02820816514679644</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01530375517904758</v>
+        <v>0.01293173339217901</v>
       </c>
       <c r="D6" t="n">
         <v>0.04386869592222259</v>
@@ -537,7 +537,7 @@
         <v>-0.02839234060633996</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01784522645175457</v>
+        <v>0.01401621662080288</v>
       </c>
       <c r="D7" t="n">
         <v>0.1392417023944478</v>
@@ -551,7 +551,7 @@
         <v>-0.02849407655437788</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01696161925792694</v>
+        <v>0.0144551582634449</v>
       </c>
       <c r="D8" t="n">
         <v>0.2375186071485852</v>
@@ -565,7 +565,7 @@
         <v>-0.02855027406923043</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01500768773257732</v>
+        <v>0.01450350880622864</v>
       </c>
       <c r="D9" t="n">
         <v>0.3260259262437482</v>
@@ -579,7 +579,7 @@
         <v>-0.02858131679047609</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0132947089150548</v>
+        <v>0.01437765080481768</v>
       </c>
       <c r="D10" t="n">
         <v>0.3870115776402003</v>
@@ -593,7 +593,7 @@
         <v>-0.02859846435553949</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01226875837892294</v>
+        <v>0.01428111549466848</v>
       </c>
       <c r="D11" t="n">
         <v>0.4206159471286733</v>

</xml_diff>